<commit_message>
modificaciones al archivo xlsx
</commit_message>
<xml_diff>
--- a/Resultados Tarea 1.xlsx
+++ b/Resultados Tarea 1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="34">
   <si>
     <t>2^2</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Error Estándar</t>
+  </si>
+  <si>
+    <t>BMH</t>
+  </si>
+  <si>
+    <t>KMP</t>
+  </si>
+  <si>
+    <t>BF</t>
   </si>
   <si>
     <t>Fuerza Bruta</t>
@@ -175,7 +184,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -195,7 +204,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1300,6 +1308,65 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(RealDNA!$D$6,RealDNA!$F$6,RealDNA!$H$6,RealDNA!$J$6,RealDNA!$L$6,RealDNA!$N$6)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>4.0922851347324754E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.1004222198753717E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.0938754251100317E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.084644206582248E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.0949901551636707E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.0941411846492134E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(RealDNA!$D$7,RealDNA!$F$7,RealDNA!$H$7,RealDNA!$J$7,RealDNA!$L$7,RealDNA!$N$7)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>-4.0922851347324754E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-4.1004222198753717E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>-4.0938754251100317E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-4.084644206582248E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-4.0949901551636707E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>-4.0941411846492134E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(RealDNA!$D$1,RealDNA!$F$1,RealDNA!$H$1,RealDNA!$J$1,RealDNA!$L$1,RealDNA!$N$1)</c:f>
@@ -1369,6 +1436,65 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(RealDNA!$D$11,RealDNA!$F$11,RealDNA!$H$11,RealDNA!$J$11,RealDNA!$L$11,RealDNA!$N$11)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>4.133243868210232E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.6062646184477814E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.5947559124983423E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.5749590777673982E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.5708056468855588E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.5728327781614104E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(RealDNA!$D$12,RealDNA!$F$12,RealDNA!$H$12,RealDNA!$J$12,RealDNA!$L$12,RealDNA!$N$12)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>-4.133243868210232E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-5.6062646184477814E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>-1.5947559124983423E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-1.5749590777673982E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-1.5708056468855588E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>-1.5728327781614104E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(RealDNA!$D$1,RealDNA!$F$1,RealDNA!$H$1,RealDNA!$J$1,RealDNA!$L$1,RealDNA!$N$1)</c:f>
@@ -1438,6 +1564,65 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(RealDNA!$D$16,RealDNA!$F$16,RealDNA!$H$16,RealDNA!$J$16,RealDNA!$L$16,RealDNA!$N$16)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>3.7277415577186246E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.3798463111248773E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.0976447899761092E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.0969411404434151E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.0995642291880331E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1000450078339406E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(RealDNA!$D$17,RealDNA!$F$17,RealDNA!$H$17,RealDNA!$J$17,RealDNA!$L$17,RealDNA!$N$17)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>-3.7277415577186246E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-4.3798463111248773E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>-1.0976447899761092E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-1.0969411404434151E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-1.0995642291880331E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>-1.1000450078339406E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(RealDNA!$D$1,RealDNA!$F$1,RealDNA!$H$1,RealDNA!$J$1,RealDNA!$L$1,RealDNA!$N$1)</c:f>
@@ -1610,6 +1795,65 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(RealDNA!$E$6,RealDNA!$G$6,RealDNA!$I$6,RealDNA!$K$6,RealDNA!$M$6,RealDNA!$O$6)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>211.48831113594463</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>222.74821800026373</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>222.37768914449595</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>220.50547162443428</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>221.74415845517319</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>220.88924547549203</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(RealDNA!$E$7,RealDNA!$G$7,RealDNA!$I$7,RealDNA!$K$7,RealDNA!$M$7,RealDNA!$O$7)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>-211.48831113594463</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-222.74821800026373</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>-222.37768914449595</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-220.50547162443428</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-221.74415845517319</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>-220.88924547549203</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(RealDNA!$E$1,RealDNA!$G$1,RealDNA!$I$1,RealDNA!$K$1,RealDNA!$M$1,RealDNA!$O$1)</c:f>
@@ -1679,6 +1923,65 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(RealDNA!$E$11,RealDNA!$G$11,RealDNA!$I$11,RealDNA!$K$11,RealDNA!$M$11,RealDNA!$O$11)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>7.6785144846467057</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1094.2474545851101</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3696.4744132690116</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3643.0761596785519</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3633.6906961513268</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3635.8280343489805</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(RealDNA!$E$12,RealDNA!$G$12,RealDNA!$I$12,RealDNA!$K$12,RealDNA!$M$12,RealDNA!$O$12)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>-7.6785144846467057</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-1094.2474545851101</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>-3696.4744132690116</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-3643.0761596785519</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-3633.6906961513268</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>-3635.8280343489805</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(RealDNA!$E$1,RealDNA!$G$1,RealDNA!$I$1,RealDNA!$K$1,RealDNA!$M$1,RealDNA!$O$1)</c:f>
@@ -1748,6 +2051,65 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(RealDNA!$E$16,RealDNA!$G$16,RealDNA!$I$16,RealDNA!$K$16,RealDNA!$M$16,RealDNA!$O$16)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>14.507925918211514</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1103.4590617052795</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3611.2501810035064</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3571.6089374525964</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3572.6118421952274</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3574.6484734759065</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(RealDNA!$E$17,RealDNA!$G$17,RealDNA!$I$17,RealDNA!$K$17,RealDNA!$M$17,RealDNA!$O$17)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>-14.507925918211514</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-1103.4590617052795</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>-3611.2501810035064</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-3571.6089374525964</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-3572.6118421952274</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>-3574.6484734759065</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(RealDNA!$E$1,RealDNA!$G$1,RealDNA!$I$1,RealDNA!$K$1,RealDNA!$M$1,RealDNA!$O$1)</c:f>
@@ -1857,6 +2219,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr u="none"/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -2334,7 +2706,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>16</v>
@@ -2473,7 +2845,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>16</v>
@@ -2612,7 +2984,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>16</v>
@@ -2800,7 +3172,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>16</v>
@@ -2937,7 +3309,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>16</v>
@@ -3083,7 +3455,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>16</v>
@@ -3225,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3282,46 +3654,46 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="16"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>4.7935800000000599</v>
@@ -3403,7 +3775,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>0.45753138722868503</v>
@@ -3447,110 +3819,110 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <f>D5/SQRT(50000)</f>
-        <v>2.0461425673662377E-3</v>
+        <f>2*D5/SQRT(50000)</f>
+        <v>4.0922851347324754E-3</v>
       </c>
       <c r="E6">
-        <f>E5/SQRT(50000)</f>
-        <v>105.74415556797231</v>
+        <f t="shared" ref="E6:O6" si="0">2*E5/SQRT(50000)</f>
+        <v>211.48831113594463</v>
       </c>
       <c r="F6">
-        <f>F5/SQRT(50000)</f>
-        <v>2.0502111099376858E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.1004222198753717E-3</v>
       </c>
       <c r="G6">
-        <f>G5/SQRT(50000)</f>
-        <v>111.37410900013187</v>
+        <f t="shared" si="0"/>
+        <v>222.74821800026373</v>
       </c>
       <c r="H6">
-        <f>H5/SQRT(50000)</f>
-        <v>2.0469377125550158E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.0938754251100317E-3</v>
       </c>
       <c r="I6">
-        <f>I5/SQRT(50000)</f>
-        <v>111.18884457224797</v>
+        <f t="shared" si="0"/>
+        <v>222.37768914449595</v>
       </c>
       <c r="J6">
-        <f>J5/SQRT(50000)</f>
-        <v>2.042322103291124E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.084644206582248E-3</v>
       </c>
       <c r="K6">
-        <f>K5/SQRT(50000)</f>
-        <v>110.25273581221714</v>
+        <f t="shared" si="0"/>
+        <v>220.50547162443428</v>
       </c>
       <c r="L6">
-        <f>L5/SQRT(50000)</f>
-        <v>2.0474950775818354E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.0949901551636707E-3</v>
       </c>
       <c r="M6">
-        <f>M5/SQRT(50000)</f>
-        <v>110.8720792275866</v>
+        <f t="shared" si="0"/>
+        <v>221.74415845517319</v>
       </c>
       <c r="N6">
-        <f>N5/SQRT(50000)</f>
-        <v>2.0470705923246067E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.0941411846492134E-3</v>
       </c>
       <c r="O6">
-        <f>O5/SQRT(50000)</f>
-        <v>110.44462273774602</v>
+        <f t="shared" si="0"/>
+        <v>220.88924547549203</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <f>-D6</f>
-        <v>-2.0461425673662377E-3</v>
+        <v>-4.0922851347324754E-3</v>
       </c>
       <c r="E7">
         <f>-E6</f>
-        <v>-105.74415556797231</v>
+        <v>-211.48831113594463</v>
       </c>
       <c r="F7">
         <f>-F6</f>
-        <v>-2.0502111099376858E-3</v>
+        <v>-4.1004222198753717E-3</v>
       </c>
       <c r="G7">
         <f>-G6</f>
-        <v>-111.37410900013187</v>
+        <v>-222.74821800026373</v>
       </c>
       <c r="H7">
         <f>-H6</f>
-        <v>-2.0469377125550158E-3</v>
+        <v>-4.0938754251100317E-3</v>
       </c>
       <c r="I7">
         <f>-I6</f>
-        <v>-111.18884457224797</v>
+        <v>-222.37768914449595</v>
       </c>
       <c r="J7">
         <f>-J6</f>
-        <v>-2.042322103291124E-3</v>
+        <v>-4.084644206582248E-3</v>
       </c>
       <c r="K7">
         <f>-K6</f>
-        <v>-110.25273581221714</v>
+        <v>-220.50547162443428</v>
       </c>
       <c r="L7">
         <f>-L6</f>
-        <v>-2.0474950775818354E-3</v>
+        <v>-4.0949901551636707E-3</v>
       </c>
       <c r="M7">
         <f>-M6</f>
-        <v>-110.8720792275866</v>
+        <v>-221.74415845517319</v>
       </c>
       <c r="N7">
         <f>-N6</f>
-        <v>-2.0470705923246067E-3</v>
+        <v>-4.0941411846492134E-3</v>
       </c>
       <c r="O7">
         <f>-O6</f>
-        <v>-110.44462273774602</v>
+        <v>-220.88924547549203</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>2.1400000000000099E-3</v>
@@ -3632,7 +4004,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>4.6211071284511303E-2</v>
@@ -3676,110 +4048,110 @@
         <v>20</v>
       </c>
       <c r="D11">
-        <f>D10/SQRT(50000)</f>
-        <v>2.066621934105116E-4</v>
+        <f>2*D10/SQRT(50000)</f>
+        <v>4.133243868210232E-4</v>
       </c>
       <c r="E11">
-        <f>E10/SQRT(50000)</f>
-        <v>3.8392572423233529</v>
+        <f t="shared" ref="E11:O11" si="1">2*E10/SQRT(50000)</f>
+        <v>7.6785144846467057</v>
       </c>
       <c r="F11">
-        <f>F10/SQRT(50000)</f>
-        <v>2.8031323092238907E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.6062646184477814E-3</v>
       </c>
       <c r="G11">
-        <f>G10/SQRT(50000)</f>
-        <v>547.12372729255503</v>
+        <f t="shared" si="1"/>
+        <v>1094.2474545851101</v>
       </c>
       <c r="H11">
-        <f>H10/SQRT(50000)</f>
-        <v>7.9737795624917115E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.5947559124983423E-2</v>
       </c>
       <c r="I11">
-        <f>I10/SQRT(50000)</f>
-        <v>1848.2372066345058</v>
+        <f t="shared" si="1"/>
+        <v>3696.4744132690116</v>
       </c>
       <c r="J11">
-        <f>J10/SQRT(50000)</f>
-        <v>7.8747953888369908E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.5749590777673982E-2</v>
       </c>
       <c r="K11">
-        <f>K10/SQRT(50000)</f>
-        <v>1821.538079839276</v>
+        <f t="shared" si="1"/>
+        <v>3643.0761596785519</v>
       </c>
       <c r="L11">
-        <f>L10/SQRT(50000)</f>
-        <v>7.8540282344277939E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.5708056468855588E-2</v>
       </c>
       <c r="M11">
-        <f>M10/SQRT(50000)</f>
-        <v>1816.8453480756634</v>
+        <f t="shared" si="1"/>
+        <v>3633.6906961513268</v>
       </c>
       <c r="N11">
-        <f>N10/SQRT(50000)</f>
-        <v>7.8641638908070518E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.5728327781614104E-2</v>
       </c>
       <c r="O11">
-        <f>O10/SQRT(50000)</f>
-        <v>1817.9140171744903</v>
+        <f t="shared" si="1"/>
+        <v>3635.8280343489805</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <f>-D11</f>
-        <v>-2.066621934105116E-4</v>
+        <v>-4.133243868210232E-4</v>
       </c>
       <c r="E12">
         <f>-E11</f>
-        <v>-3.8392572423233529</v>
+        <v>-7.6785144846467057</v>
       </c>
       <c r="F12">
         <f>-F11</f>
-        <v>-2.8031323092238907E-3</v>
+        <v>-5.6062646184477814E-3</v>
       </c>
       <c r="G12">
         <f>-G11</f>
-        <v>-547.12372729255503</v>
+        <v>-1094.2474545851101</v>
       </c>
       <c r="H12">
         <f>-H11</f>
-        <v>-7.9737795624917115E-3</v>
+        <v>-1.5947559124983423E-2</v>
       </c>
       <c r="I12">
         <f>-I11</f>
-        <v>-1848.2372066345058</v>
+        <v>-3696.4744132690116</v>
       </c>
       <c r="J12">
         <f>-J11</f>
-        <v>-7.8747953888369908E-3</v>
+        <v>-1.5749590777673982E-2</v>
       </c>
       <c r="K12">
         <f>-K11</f>
-        <v>-1821.538079839276</v>
+        <v>-3643.0761596785519</v>
       </c>
       <c r="L12">
         <f>-L11</f>
-        <v>-7.8540282344277939E-3</v>
+        <v>-1.5708056468855588E-2</v>
       </c>
       <c r="M12">
         <f>-M11</f>
-        <v>-1816.8453480756634</v>
+        <v>-3633.6906961513268</v>
       </c>
       <c r="N12">
         <f>-N11</f>
-        <v>-7.8641638908070518E-3</v>
+        <v>-1.5728327781614104E-2</v>
       </c>
       <c r="O12">
         <f>-O11</f>
-        <v>-1817.9140171744903</v>
+        <v>-3635.8280343489805</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13">
         <v>1.74E-3</v>
@@ -3862,7 +4234,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>4.1677417628049003E-2</v>
@@ -3906,105 +4278,105 @@
         <v>20</v>
       </c>
       <c r="D16">
-        <f>D15/SQRT(50000)</f>
-        <v>1.8638707788593123E-4</v>
+        <f>2*D15/SQRT(50000)</f>
+        <v>3.7277415577186246E-4</v>
       </c>
       <c r="E16">
-        <f>E15/SQRT(50000)</f>
-        <v>7.2539629591057571</v>
+        <f t="shared" ref="E16:O16" si="2">2*E15/SQRT(50000)</f>
+        <v>14.507925918211514</v>
       </c>
       <c r="F16">
-        <f>F15/SQRT(50000)</f>
-        <v>2.1899231555624387E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.3798463111248773E-3</v>
       </c>
       <c r="G16">
-        <f>G15/SQRT(50000)</f>
-        <v>551.72953085263975</v>
+        <f t="shared" si="2"/>
+        <v>1103.4590617052795</v>
       </c>
       <c r="H16">
-        <f>H15/SQRT(50000)</f>
-        <v>5.4882239498805462E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.0976447899761092E-2</v>
       </c>
       <c r="I16">
-        <f>I15/SQRT(50000)</f>
-        <v>1805.6250905017532</v>
+        <f t="shared" si="2"/>
+        <v>3611.2501810035064</v>
       </c>
       <c r="J16">
-        <f>J15/SQRT(50000)</f>
-        <v>5.4847057022170756E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.0969411404434151E-2</v>
       </c>
       <c r="K16">
-        <f>K15/SQRT(50000)</f>
-        <v>1785.8044687262982</v>
+        <f t="shared" si="2"/>
+        <v>3571.6089374525964</v>
       </c>
       <c r="L16">
-        <f>L15/SQRT(50000)</f>
-        <v>5.4978211459401653E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.0995642291880331E-2</v>
       </c>
       <c r="M16">
-        <f>M15/SQRT(50000)</f>
-        <v>1786.3059210976137</v>
+        <f t="shared" si="2"/>
+        <v>3572.6118421952274</v>
       </c>
       <c r="N16">
-        <f>N15/SQRT(50000)</f>
-        <v>5.5002250391697032E-3</v>
-      </c>
-      <c r="O16" s="17">
-        <f>O15/SQRT(50000)</f>
-        <v>1787.3242367379532</v>
+        <f t="shared" si="2"/>
+        <v>1.1000450078339406E-2</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>3574.6484734759065</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <f>-D16</f>
-        <v>-1.8638707788593123E-4</v>
+        <v>-3.7277415577186246E-4</v>
       </c>
       <c r="E17">
         <f>-E16</f>
-        <v>-7.2539629591057571</v>
+        <v>-14.507925918211514</v>
       </c>
       <c r="F17">
         <f>-F16</f>
-        <v>-2.1899231555624387E-3</v>
+        <v>-4.3798463111248773E-3</v>
       </c>
       <c r="G17">
         <f>-G16</f>
-        <v>-551.72953085263975</v>
+        <v>-1103.4590617052795</v>
       </c>
       <c r="H17">
         <f>-H16</f>
-        <v>-5.4882239498805462E-3</v>
+        <v>-1.0976447899761092E-2</v>
       </c>
       <c r="I17">
         <f>-I16</f>
-        <v>-1805.6250905017532</v>
+        <v>-3611.2501810035064</v>
       </c>
       <c r="J17">
         <f>-J16</f>
-        <v>-5.4847057022170756E-3</v>
+        <v>-1.0969411404434151E-2</v>
       </c>
       <c r="K17">
         <f>-K16</f>
-        <v>-1785.8044687262982</v>
+        <v>-3571.6089374525964</v>
       </c>
       <c r="L17">
         <f>-L16</f>
-        <v>-5.4978211459401653E-3</v>
+        <v>-1.0995642291880331E-2</v>
       </c>
       <c r="M17">
         <f>-M16</f>
-        <v>-1786.3059210976137</v>
+        <v>-3572.6118421952274</v>
       </c>
       <c r="N17">
         <f>-N16</f>
-        <v>-5.5002250391697032E-3</v>
+        <v>-1.1000450078339406E-2</v>
       </c>
       <c r="O17">
         <f>-O16</f>
-        <v>-1787.3242367379532</v>
+        <v>-3574.6484734759065</v>
       </c>
     </row>
   </sheetData>
@@ -4016,10 +4388,765 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>5.09295999999995</v>
+      </c>
+      <c r="D2">
+        <v>1392772.0728799901</v>
+      </c>
+      <c r="E2">
+        <v>5.0859199999999696</v>
+      </c>
+      <c r="F2">
+        <v>1398202.1531400101</v>
+      </c>
+      <c r="G2">
+        <v>5.0933000000000099</v>
+      </c>
+      <c r="H2">
+        <v>1398230.5447</v>
+      </c>
+      <c r="I2">
+        <v>5.0886799999999699</v>
+      </c>
+      <c r="J2">
+        <v>1398220.6872799899</v>
+      </c>
+      <c r="K2">
+        <v>5.0913200000000298</v>
+      </c>
+      <c r="L2">
+        <v>1398209.5757800001</v>
+      </c>
+      <c r="M2">
+        <v>5.0912199999999297</v>
+      </c>
+      <c r="N2">
+        <v>1398192.9505399901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>0.21420272245444899</v>
+      </c>
+      <c r="D3">
+        <v>599741.73872327898</v>
+      </c>
+      <c r="E3">
+        <v>0.21514205644112899</v>
+      </c>
+      <c r="F3">
+        <v>652244.704542247</v>
+      </c>
+      <c r="G3">
+        <v>0.21911949238984599</v>
+      </c>
+      <c r="H3">
+        <v>647646.39312980894</v>
+      </c>
+      <c r="I3">
+        <v>0.213860134802698</v>
+      </c>
+      <c r="J3">
+        <v>653818.924064619</v>
+      </c>
+      <c r="K3">
+        <v>0.21730500370007499</v>
+      </c>
+      <c r="L3">
+        <v>653497.21812175994</v>
+      </c>
+      <c r="M3">
+        <v>0.21446320086401599</v>
+      </c>
+      <c r="N3">
+        <v>650190.31237996102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>0.462820399782085</v>
+      </c>
+      <c r="D4">
+        <v>774.42994436119204</v>
+      </c>
+      <c r="E4">
+        <v>0.463834082879998</v>
+      </c>
+      <c r="F4">
+        <v>807.61668168893505</v>
+      </c>
+      <c r="G4">
+        <v>0.46810201066631402</v>
+      </c>
+      <c r="H4">
+        <v>804.76480609542602</v>
+      </c>
+      <c r="I4">
+        <v>0.46245014304538601</v>
+      </c>
+      <c r="J4">
+        <v>808.59070243518102</v>
+      </c>
+      <c r="K4">
+        <v>0.46615984779909497</v>
+      </c>
+      <c r="L4">
+        <v>808.391747930272</v>
+      </c>
+      <c r="M4">
+        <v>0.46310171762153501</v>
+      </c>
+      <c r="N4">
+        <v>806.34379291959601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <f>2*C4/SQRT(50000)</f>
+        <v>4.1395915011454834E-3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:N5" si="0">2*D4/SQRT(50000)</f>
+        <v>6.9267119976120215</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>4.1486581584037879E-3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>7.2235432000770734</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>4.1868316650168387E-3</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>7.1980352493152386</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>4.1362798242159391E-3</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>7.2322551064774778</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>4.1694604322389285E-3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>7.2304756032878528</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>4.142107684394658E-3</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>7.2121581368129215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <f>-C5</f>
+        <v>-4.1395915011454834E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:N6" si="1">-D5</f>
+        <v>-6.9267119976120215</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>-4.1486581584037879E-3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>-7.2235432000770734</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>-4.1868316650168387E-3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>-7.1980352493152386</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-4.1362798242159391E-3</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>-7.2322551064774778</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>-4.1694604322389285E-3</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>-7.2304756032878528</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>-4.142107684394658E-3</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>-7.2121581368129215</v>
+      </c>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>1.8400000000000001E-3</v>
+      </c>
+      <c r="D7">
+        <v>386.68885999999799</v>
+      </c>
+      <c r="E7">
+        <v>0.377159999999997</v>
+      </c>
+      <c r="F7">
+        <v>87207.884739999296</v>
+      </c>
+      <c r="G7">
+        <v>3.1638799999999998</v>
+      </c>
+      <c r="H7">
+        <v>730363.73114000598</v>
+      </c>
+      <c r="I7">
+        <v>3.18213999999998</v>
+      </c>
+      <c r="J7">
+        <v>734605.98251999705</v>
+      </c>
+      <c r="K7">
+        <v>3.1809599999999998</v>
+      </c>
+      <c r="L7">
+        <v>733891.18229999905</v>
+      </c>
+      <c r="M7">
+        <v>3.18203999999999</v>
+      </c>
+      <c r="N7">
+        <v>734424.42971999699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>1.8366511330226501E-3</v>
+      </c>
+      <c r="D8">
+        <v>147687.063953178</v>
+      </c>
+      <c r="E8">
+        <v>0.29231618072361398</v>
+      </c>
+      <c r="F8" s="12">
+        <v>7707811098.0828304</v>
+      </c>
+      <c r="G8">
+        <v>3.4244118338366598</v>
+      </c>
+      <c r="H8" s="12">
+        <v>174828398533.69601</v>
+      </c>
+      <c r="I8">
+        <v>3.4131132826656199</v>
+      </c>
+      <c r="J8" s="12">
+        <v>174402425025.84201</v>
+      </c>
+      <c r="K8">
+        <v>3.4122017224344501</v>
+      </c>
+      <c r="L8" s="12">
+        <v>173908381835.944</v>
+      </c>
+      <c r="M8">
+        <v>3.4264899681994199</v>
+      </c>
+      <c r="N8" s="12">
+        <v>174609021929.42599</v>
+      </c>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>4.2856167969414299E-2</v>
+      </c>
+      <c r="D9">
+        <v>384.30074675074201</v>
+      </c>
+      <c r="E9">
+        <v>0.54066272363055901</v>
+      </c>
+      <c r="F9">
+        <v>87794.140454148903</v>
+      </c>
+      <c r="G9">
+        <v>1.8505166397081301</v>
+      </c>
+      <c r="H9">
+        <v>418124.85998047999</v>
+      </c>
+      <c r="I9">
+        <v>1.8474613074880899</v>
+      </c>
+      <c r="J9">
+        <v>417615.16378819599</v>
+      </c>
+      <c r="K9">
+        <v>1.8472145848369701</v>
+      </c>
+      <c r="L9">
+        <v>417023.238963902</v>
+      </c>
+      <c r="M9">
+        <v>1.85107805567443</v>
+      </c>
+      <c r="N9">
+        <v>417862.44378913299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <f>2*C9/SQRT(50000)</f>
+        <v>3.8331721933903802E-4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:N10" si="2">2*D9/SQRT(50000)</f>
+        <v>3.4372903741543621</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>4.835834411752447E-3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>785.25466432656481</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>1.6551523999527463E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>3739.8224399957385</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>1.652419627737604E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>3735.2635786604592</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>1.6521989522898069E-2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>3729.9692420816955</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>1.6556545456584661E-2</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>3737.4753182267445</v>
+      </c>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <f>-C10</f>
+        <v>-3.8331721933903802E-4</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:N11" si="3">-D10</f>
+        <v>-3.4372903741543621</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>-4.835834411752447E-3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>-785.25466432656481</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>-1.6551523999527463E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>-3739.8224399957385</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>-1.652419627737604E-2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>-3735.2635786604592</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>-1.6521989522898069E-2</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>-3729.9692420816955</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>-1.6556545456584661E-2</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>-3737.4753182267445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>1.55999999999999E-3</v>
+      </c>
+      <c r="D12">
+        <v>428.827259999999</v>
+      </c>
+      <c r="E12">
+        <v>0.25354000000000099</v>
+      </c>
+      <c r="F12">
+        <v>87362.785799999794</v>
+      </c>
+      <c r="G12">
+        <v>2.0094600000000198</v>
+      </c>
+      <c r="H12">
+        <v>719050.991159998</v>
+      </c>
+      <c r="I12">
+        <v>2.0182399999999601</v>
+      </c>
+      <c r="J12">
+        <v>724877.47230000701</v>
+      </c>
+      <c r="K12">
+        <v>2.0028599999999899</v>
+      </c>
+      <c r="L12">
+        <v>721796.29705999803</v>
+      </c>
+      <c r="M12">
+        <v>2.0144200000000199</v>
+      </c>
+      <c r="N12">
+        <v>724106.293119999</v>
+      </c>
+      <c r="P12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>1.55759755195102E-3</v>
+      </c>
+      <c r="D13">
+        <v>191983.01304115399</v>
+      </c>
+      <c r="E13">
+        <v>0.20062148082961501</v>
+      </c>
+      <c r="F13" s="12">
+        <v>7663927874.4538698</v>
+      </c>
+      <c r="G13">
+        <v>1.75724565331305</v>
+      </c>
+      <c r="H13" s="12">
+        <v>179719665060.327</v>
+      </c>
+      <c r="I13">
+        <v>1.7619025404508</v>
+      </c>
+      <c r="J13" s="12">
+        <v>178246410009.427</v>
+      </c>
+      <c r="K13">
+        <v>1.7337264949299001</v>
+      </c>
+      <c r="L13" s="12">
+        <v>177944199855.276</v>
+      </c>
+      <c r="M13">
+        <v>1.76648739334785</v>
+      </c>
+      <c r="N13" s="12">
+        <v>178814272172.47198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>3.9466410426475598E-2</v>
+      </c>
+      <c r="D14">
+        <v>438.158661949247</v>
+      </c>
+      <c r="E14">
+        <v>0.44790789324325903</v>
+      </c>
+      <c r="F14">
+        <v>87543.862574448198</v>
+      </c>
+      <c r="G14">
+        <v>1.3256114262154799</v>
+      </c>
+      <c r="H14">
+        <v>423933.562082936</v>
+      </c>
+      <c r="I14">
+        <v>1.3273667693786799</v>
+      </c>
+      <c r="J14">
+        <v>422192.38506802497</v>
+      </c>
+      <c r="K14">
+        <v>1.3167104825776601</v>
+      </c>
+      <c r="L14">
+        <v>421834.32749751001</v>
+      </c>
+      <c r="M14">
+        <v>1.3290926955437801</v>
+      </c>
+      <c r="N14">
+        <v>422864.36616540799</v>
+      </c>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <f>2*C14/SQRT(50000)</f>
+        <v>3.5299830616602362E-4</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:N15" si="4">2*D14/SQRT(50000)</f>
+        <v>3.9190102121954675</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>4.0062099878025838E-3</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>783.01611091746372</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>1.1856629043073039E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>3791.7770510442888</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>1.1872329309620058E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>3776.2034903794843</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>1.1777016582920801E-2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="4"/>
+        <v>3773.0009261093646</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>1.1887766462537296E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>3782.2138720328576</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <f>-C15</f>
+        <v>-3.5299830616602362E-4</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:N16" si="5">-D15</f>
+        <v>-3.9190102121954675</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="5"/>
+        <v>-4.0062099878025838E-3</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="5"/>
+        <v>-783.01611091746372</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>-1.1856629043073039E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>-3791.7770510442888</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>-1.1872329309620058E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>-3776.2034903794843</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>-1.1777016582920801E-2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="5"/>
+        <v>-3773.0009261093646</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="5"/>
+        <v>-1.1887766462537296E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>-3782.2138720328576</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:S1"/>
+      <selection sqref="A1:D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4035,13 +5162,13 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
         <v>16</v>
@@ -4050,13 +5177,13 @@
         <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O1" t="s">
         <v>16</v>
@@ -4065,13 +5192,13 @@
         <v>17</v>
       </c>
       <c r="Q1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="S1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4084,13 +5211,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5.09295999999995</v>
+        <v>2.88714</v>
       </c>
       <c r="C3">
-        <v>0.21420272245444899</v>
+        <v>0.39141044860897201</v>
       </c>
       <c r="D3">
-        <v>0.462820399782085</v>
+        <v>0.62562804333643196</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -4098,13 +5225,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1392772.0728799901</v>
-      </c>
-      <c r="C4">
-        <v>599741.73872327898</v>
+        <v>1085113.01364</v>
+      </c>
+      <c r="C4" s="12">
+        <v>2792382558.1357002</v>
       </c>
       <c r="D4">
-        <v>774.42994436119204</v>
+        <v>52842.999140242799</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -4117,13 +5244,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1.8400000000000001E-3</v>
+        <v>0.101959999999999</v>
       </c>
       <c r="C6">
-        <v>1.8366511330226501E-3</v>
+        <v>0.12964675133502501</v>
       </c>
       <c r="D6">
-        <v>4.2856167969414299E-2</v>
+        <v>0.36006492655495498</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -4131,13 +5258,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>386.68885999999799</v>
-      </c>
-      <c r="C7">
-        <v>147687.063953178</v>
+        <v>39886.780620000398</v>
+      </c>
+      <c r="C7" s="12">
+        <v>13381431632.130899</v>
       </c>
       <c r="D7">
-        <v>384.30074675074201</v>
+        <v>115678.13809069899</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -4150,13 +5277,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.55999999999999E-3</v>
+        <v>0.11581999999999899</v>
       </c>
       <c r="C9">
-        <v>1.55759755195102E-3</v>
+        <v>0.15784888457769</v>
       </c>
       <c r="D9">
-        <v>3.9466410426475598E-2</v>
+        <v>0.39730200676272798</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -4164,13 +5291,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>428.827259999999</v>
-      </c>
-      <c r="C10">
-        <v>191983.01304115399</v>
+        <v>51133.254540000104</v>
+      </c>
+      <c r="C10" s="12">
+        <v>21889235390.262798</v>
       </c>
       <c r="D10">
-        <v>438.158661949247</v>
+        <v>147950.111153262</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -4188,13 +5315,13 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>5.0859199999999696</v>
+        <v>2.8904799999999899</v>
       </c>
       <c r="C13">
-        <v>0.21514205644112899</v>
+        <v>0.392693223464464</v>
       </c>
       <c r="D13">
-        <v>0.463834082879998</v>
+        <v>0.62665239444564802</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -4202,13 +5329,13 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <v>1398202.1531400101</v>
-      </c>
-      <c r="C14">
-        <v>652244.704542247</v>
+        <v>1086923.77375999</v>
+      </c>
+      <c r="C14" s="12">
+        <v>3033888525.2679901</v>
       </c>
       <c r="D14">
-        <v>807.61668168893505</v>
+        <v>55080.745503923499</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -4221,13 +5348,13 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>0.377159999999997</v>
+        <v>0.83838000000000001</v>
       </c>
       <c r="C16">
-        <v>0.29231618072361398</v>
+        <v>0.95571808996180696</v>
       </c>
       <c r="D16">
-        <v>0.54066272363055901</v>
+        <v>0.97760835203153096</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4235,13 +5362,13 @@
         <v>6</v>
       </c>
       <c r="B17">
-        <v>87207.884739999296</v>
+        <v>310636.147740004</v>
       </c>
       <c r="C17" s="12">
-        <v>7707811098.0828304</v>
+        <v>105240515949.242</v>
       </c>
       <c r="D17">
-        <v>87794.140454148903</v>
+        <v>324407.94680346898</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4254,13 +5381,13 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <v>0.25354000000000099</v>
+        <v>0.61099999999999799</v>
       </c>
       <c r="C19">
-        <v>0.20062148082961501</v>
+        <v>0.54208984179683495</v>
       </c>
       <c r="D19">
-        <v>0.44790789324325903</v>
+        <v>0.73626750695439103</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4268,13 +5395,13 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>87362.785799999794</v>
+        <v>344751.70803999901</v>
       </c>
       <c r="C20" s="12">
-        <v>7663927874.4538698</v>
+        <v>129396838028.784</v>
       </c>
       <c r="D20">
-        <v>87543.862574448198</v>
+        <v>359717.71992603398</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -4292,13 +5419,13 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>5.0933000000000099</v>
+        <v>2.8906999999999901</v>
       </c>
       <c r="C23">
-        <v>0.21911949238984599</v>
+        <v>0.397761465229304</v>
       </c>
       <c r="D23">
-        <v>0.46810201066631402</v>
+        <v>0.63068333197358595</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4306,13 +5433,13 @@
         <v>3</v>
       </c>
       <c r="B24">
-        <v>1398230.5447</v>
-      </c>
-      <c r="C24">
-        <v>647646.39312980894</v>
+        <v>1087000.31072001</v>
+      </c>
+      <c r="C24" s="12">
+        <v>3060357355.0716701</v>
       </c>
       <c r="D24">
-        <v>804.76480609542602</v>
+        <v>55320.496699430201</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4325,13 +5452,13 @@
         <v>5</v>
       </c>
       <c r="B26">
-        <v>3.1638799999999998</v>
+        <v>1.4307999999999901</v>
       </c>
       <c r="C26">
-        <v>3.4244118338366598</v>
+        <v>1.1201937638752699</v>
       </c>
       <c r="D26">
-        <v>1.8505166397081301</v>
+        <v>1.0583920652930401</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4339,13 +5466,13 @@
         <v>6</v>
       </c>
       <c r="B27">
-        <v>730363.73114000598</v>
+        <v>519315.28939999902</v>
       </c>
       <c r="C27" s="12">
-        <v>174828398533.69601</v>
+        <v>107202359569.51801</v>
       </c>
       <c r="D27">
-        <v>418124.85998047999</v>
+        <v>327417.71419628197</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4358,13 +5485,13 @@
         <v>8</v>
       </c>
       <c r="B29">
-        <v>2.0094600000000198</v>
+        <v>0.87898000000000198</v>
       </c>
       <c r="C29">
-        <v>1.75724565331305</v>
+        <v>0.480743774475487</v>
       </c>
       <c r="D29">
-        <v>1.3256114262154799</v>
+        <v>0.69335688824406105</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4372,13 +5499,13 @@
         <v>9</v>
       </c>
       <c r="B30">
-        <v>719050.991159998</v>
+        <v>532796.18673999805</v>
       </c>
       <c r="C30" s="12">
-        <v>179719665060.327</v>
+        <v>112086358637.27901</v>
       </c>
       <c r="D30">
-        <v>423933.562082936</v>
+        <v>334793.00864456501</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4396,13 +5523,13 @@
         <v>2</v>
       </c>
       <c r="B33">
-        <v>5.0886799999999699</v>
+        <v>2.8907599999999798</v>
       </c>
       <c r="C33">
-        <v>0.213860134802698</v>
+        <v>0.39387449988999601</v>
       </c>
       <c r="D33">
-        <v>0.46245014304538601</v>
+        <v>0.62759421594689402</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4410,13 +5537,13 @@
         <v>3</v>
       </c>
       <c r="B34">
-        <v>1398220.6872799899</v>
-      </c>
-      <c r="C34">
-        <v>653818.924064619</v>
+        <v>1086849.5624599999</v>
+      </c>
+      <c r="C34" s="12">
+        <v>3030224253.03896</v>
       </c>
       <c r="D34">
-        <v>808.59070243518102</v>
+        <v>55047.472721633298</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4429,13 +5556,13 @@
         <v>5</v>
       </c>
       <c r="B36">
-        <v>3.18213999999998</v>
+        <v>1.4957400000000001</v>
       </c>
       <c r="C36">
-        <v>3.4131132826656199</v>
+        <v>1.08304351327026</v>
       </c>
       <c r="D36">
-        <v>1.8474613074880899</v>
+        <v>1.0406937653653201</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4443,13 +5570,13 @@
         <v>6</v>
       </c>
       <c r="B37">
-        <v>734605.98251999705</v>
+        <v>542355.34852000303</v>
       </c>
       <c r="C37" s="12">
-        <v>174402425025.84201</v>
+        <v>100887619263.65601</v>
       </c>
       <c r="D37">
-        <v>417615.16378819599</v>
+        <v>317628.11472483998</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4462,13 +5589,13 @@
         <v>8</v>
       </c>
       <c r="B39">
-        <v>2.0182399999999601</v>
+        <v>0.74107999999999397</v>
       </c>
       <c r="C39">
-        <v>1.7619025404508</v>
+        <v>0.34952742414848198</v>
       </c>
       <c r="D39">
-        <v>1.3273667693786799</v>
+        <v>0.59120844390830696</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,13 +5603,13 @@
         <v>9</v>
       </c>
       <c r="B40">
-        <v>724877.47230000701</v>
+        <v>540301.38448000397</v>
       </c>
       <c r="C40" s="12">
-        <v>178246410009.427</v>
+        <v>97590780608.7892</v>
       </c>
       <c r="D40">
-        <v>422192.38506802497</v>
+        <v>312395.23141173099</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4500,13 +5627,13 @@
         <v>2</v>
       </c>
       <c r="B43">
-        <v>5.0913200000000298</v>
+        <v>2.88891999999997</v>
       </c>
       <c r="C43">
-        <v>0.21730500370007499</v>
+        <v>0.39306909498190201</v>
       </c>
       <c r="D43">
-        <v>0.46615984779909497</v>
+        <v>0.62695222703320996</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4514,13 +5641,13 @@
         <v>3</v>
       </c>
       <c r="B44">
-        <v>1398209.5757800001</v>
-      </c>
-      <c r="C44">
-        <v>653497.21812175994</v>
+        <v>1086605.3466799899</v>
+      </c>
+      <c r="C44" s="12">
+        <v>3015689163.7546802</v>
       </c>
       <c r="D44">
-        <v>808.391747930272</v>
+        <v>54915.290800966199</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4533,13 +5660,13 @@
         <v>5</v>
       </c>
       <c r="B46">
-        <v>3.1809599999999998</v>
+        <v>1.4999399999999901</v>
       </c>
       <c r="C46">
-        <v>3.4122017224344501</v>
+        <v>1.0802616016320199</v>
       </c>
       <c r="D46">
-        <v>1.8472145848369701</v>
+        <v>1.0393563400643799</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4547,13 +5674,13 @@
         <v>6</v>
       </c>
       <c r="B47">
-        <v>733891.18229999905</v>
+        <v>544105.80775999697</v>
       </c>
       <c r="C47" s="12">
-        <v>173908381835.944</v>
+        <v>100464265118.071</v>
       </c>
       <c r="D47">
-        <v>417023.238963902</v>
+        <v>316960.98358957499</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,13 +5693,13 @@
         <v>8</v>
       </c>
       <c r="B49">
-        <v>2.0028599999999899</v>
+        <v>0.63603999999999195</v>
       </c>
       <c r="C49">
-        <v>1.7337264949299001</v>
+        <v>0.29221896277925402</v>
       </c>
       <c r="D49">
-        <v>1.3167104825776601</v>
+        <v>0.54057280987786804</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4580,13 +5707,13 @@
         <v>9</v>
       </c>
       <c r="B50">
-        <v>721796.29705999803</v>
+        <v>530588.46972000401</v>
       </c>
       <c r="C50" s="12">
-        <v>177944199855.276</v>
+        <v>94548217005.436905</v>
       </c>
       <c r="D50">
-        <v>421834.32749751001</v>
+        <v>307486.93794279598</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4604,13 +5731,13 @@
         <v>2</v>
       </c>
       <c r="B53">
-        <v>5.0912199999999297</v>
+        <v>2.89455999999999</v>
       </c>
       <c r="C53">
-        <v>0.21446320086401599</v>
+        <v>0.39657033780675599</v>
       </c>
       <c r="D53">
-        <v>0.46310171762153501</v>
+        <v>0.62973830898775396</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4618,13 +5745,13 @@
         <v>3</v>
       </c>
       <c r="B54">
-        <v>1398192.9505399901</v>
-      </c>
-      <c r="C54">
-        <v>650190.31237996102</v>
+        <v>1087122.94056</v>
+      </c>
+      <c r="C54" s="12">
+        <v>3035920329.5132198</v>
       </c>
       <c r="D54">
-        <v>806.34379291959601</v>
+        <v>55099.186287215001</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4637,13 +5764,13 @@
         <v>5</v>
       </c>
       <c r="B56">
-        <v>3.18203999999999</v>
+        <v>1.49769999999999</v>
       </c>
       <c r="C56">
-        <v>3.4264899681994199</v>
+        <v>1.0646160023200399</v>
       </c>
       <c r="D56">
-        <v>1.85107805567443</v>
+        <v>1.0318023077702601</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4651,13 +5778,13 @@
         <v>6</v>
       </c>
       <c r="B57">
-        <v>734424.42971999699</v>
+        <v>544345.58819999697</v>
       </c>
       <c r="C57" s="12">
-        <v>174609021929.42599</v>
+        <v>99696737850.486893</v>
       </c>
       <c r="D57">
-        <v>417862.44378913299</v>
+        <v>315747.90236910002</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4670,13 +5797,13 @@
         <v>8</v>
       </c>
       <c r="B59">
-        <v>2.0144200000000199</v>
+        <v>0.58609999999999896</v>
       </c>
       <c r="C59">
-        <v>1.76648739334785</v>
+        <v>0.26995218904378099</v>
       </c>
       <c r="D59">
-        <v>1.3290926955437801</v>
+        <v>0.51956923411974698</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4684,75 +5811,13 @@
         <v>9</v>
       </c>
       <c r="B60">
-        <v>724106.293119999</v>
+        <v>526718.12730000506</v>
       </c>
       <c r="C60" s="12">
-        <v>178814272172.47198</v>
+        <v>92862364459.065002</v>
       </c>
       <c r="D60">
-        <v>422864.36616540799</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:S1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" t="s">
-        <v>30</v>
+        <v>304733.26772616198</v>
       </c>
     </row>
   </sheetData>
@@ -4762,15 +5827,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:S1"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:S1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="E1" t="s">
         <v>16</v>
       </c>
@@ -4778,13 +5846,13 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
         <v>16</v>
@@ -4793,13 +5861,13 @@
         <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O1" t="s">
         <v>16</v>
@@ -4808,13 +5876,632 @@
         <v>17</v>
       </c>
       <c r="Q1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="S1" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.9224399999999799</v>
+      </c>
+      <c r="C3">
+        <v>0.42227289185783501</v>
+      </c>
+      <c r="D3">
+        <v>0.64982527794618405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1088329.0514</v>
+      </c>
+      <c r="C4" s="12">
+        <v>3299684638.7789698</v>
+      </c>
+      <c r="D4">
+        <v>57442.8815326927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>8.5939999999999697E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.106316442728854</v>
+      </c>
+      <c r="D6">
+        <v>0.32606202282518898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>33660.155579999999</v>
+      </c>
+      <c r="C7" s="12">
+        <v>10384864319.164101</v>
+      </c>
+      <c r="D7">
+        <v>101906.154471474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.101160000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.134729348986978</v>
+      </c>
+      <c r="D9">
+        <v>0.36705496725555697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>44558.178179999602</v>
+      </c>
+      <c r="C10" s="12">
+        <v>18192677277.2617</v>
+      </c>
+      <c r="D10">
+        <v>134880.23308573299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2.9158000000000199</v>
+      </c>
+      <c r="C13">
+        <v>0.42543886877737602</v>
+      </c>
+      <c r="D13">
+        <v>0.65225675065680699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>1088640.9209199799</v>
+      </c>
+      <c r="C14" s="12">
+        <v>3465254586.1705699</v>
+      </c>
+      <c r="D14">
+        <v>58866.413056772602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>0.98947999999999603</v>
+      </c>
+      <c r="C16">
+        <v>0.963748604572086</v>
+      </c>
+      <c r="D16">
+        <v>0.98170698508877097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>364503.04526000202</v>
+      </c>
+      <c r="C17" s="12">
+        <v>101224857284.35001</v>
+      </c>
+      <c r="D17">
+        <v>318158.54111488297</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>0.72724000000000699</v>
+      </c>
+      <c r="C19">
+        <v>0.54417286585732305</v>
+      </c>
+      <c r="D19">
+        <v>0.73768073436773596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>405780.49525999901</v>
+      </c>
+      <c r="C20" s="12">
+        <v>123566985734.827</v>
+      </c>
+      <c r="D20">
+        <v>351520.96059101098</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>2.91506000000002</v>
+      </c>
+      <c r="C23">
+        <v>0.42789375427507897</v>
+      </c>
+      <c r="D23">
+        <v>0.65413588364733399</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>1088585.11454002</v>
+      </c>
+      <c r="C24" s="12">
+        <v>3461430499.6351399</v>
+      </c>
+      <c r="D24">
+        <v>58833.923034548199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1.51118</v>
+      </c>
+      <c r="C26">
+        <v>1.12385748474969</v>
+      </c>
+      <c r="D26">
+        <v>1.0601214481132299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>542115.18453999702</v>
+      </c>
+      <c r="C27" s="12">
+        <v>101149355436.45599</v>
+      </c>
+      <c r="D27">
+        <v>318039.86453974003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>0.93543999999999605</v>
+      </c>
+      <c r="C29">
+        <v>0.46436129362587503</v>
+      </c>
+      <c r="D29">
+        <v>0.68144060168577802</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>562594.35692000203</v>
+      </c>
+      <c r="C30" s="12">
+        <v>104384818863.59399</v>
+      </c>
+      <c r="D30">
+        <v>323086.395355165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>2.9191200000000102</v>
+      </c>
+      <c r="C33">
+        <v>0.42786698293966002</v>
+      </c>
+      <c r="D33">
+        <v>0.65411542019712399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>1088966.78122</v>
+      </c>
+      <c r="C34" s="12">
+        <v>3474432130.6842599</v>
+      </c>
+      <c r="D34">
+        <v>58944.313811293599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>1.5188600000000001</v>
+      </c>
+      <c r="C36">
+        <v>1.1060664217284399</v>
+      </c>
+      <c r="D36">
+        <v>1.0516969248450001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>545739.059619996</v>
+      </c>
+      <c r="C37" s="12">
+        <v>99882196915.393494</v>
+      </c>
+      <c r="D37">
+        <v>316041.448097229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>0.74661999999999995</v>
+      </c>
+      <c r="C39">
+        <v>0.35326564091282198</v>
+      </c>
+      <c r="D39">
+        <v>0.59436154057343105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <v>541280.00101999298</v>
+      </c>
+      <c r="C40" s="12">
+        <v>97474793394.875305</v>
+      </c>
+      <c r="D40">
+        <v>312209.53443941299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43">
+        <v>2.92125999999997</v>
+      </c>
+      <c r="C43">
+        <v>0.42386848976979802</v>
+      </c>
+      <c r="D43">
+        <v>0.651051833397156</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>1089275.15013999</v>
+      </c>
+      <c r="C44" s="12">
+        <v>3475586129.7508798</v>
+      </c>
+      <c r="D44">
+        <v>58954.101890800397</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>1.52453999999999</v>
+      </c>
+      <c r="C46">
+        <v>1.12326025360507</v>
+      </c>
+      <c r="D46">
+        <v>1.0598397301503</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>546425.16065999796</v>
+      </c>
+      <c r="C47" s="12">
+        <v>100536221374.80099</v>
+      </c>
+      <c r="D47">
+        <v>317074.47291575099</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49">
+        <v>0.64009999999999501</v>
+      </c>
+      <c r="C49">
+        <v>0.29765794315886202</v>
+      </c>
+      <c r="D49">
+        <v>0.54558037277642402</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50">
+        <v>530614.88959999697</v>
+      </c>
+      <c r="C50" s="12">
+        <v>94648524767.562393</v>
+      </c>
+      <c r="D50">
+        <v>307650.003685295</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>2.9150399999999799</v>
+      </c>
+      <c r="C53">
+        <v>0.420230203004055</v>
+      </c>
+      <c r="D53">
+        <v>0.64825165098444204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>1088713.1937599999</v>
+      </c>
+      <c r="C54" s="12">
+        <v>3437185446.3453102</v>
+      </c>
+      <c r="D54">
+        <v>58627.514413842502</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>1.52464</v>
+      </c>
+      <c r="C56">
+        <v>1.1251753739074699</v>
+      </c>
+      <c r="D56">
+        <v>1.06074284061099</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57">
+        <v>546296.18840000301</v>
+      </c>
+      <c r="C57" s="12">
+        <v>100677926034.935</v>
+      </c>
+      <c r="D57">
+        <v>317297.85066233203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59">
+        <v>0.59240000000000204</v>
+      </c>
+      <c r="C59">
+        <v>0.275147742954859</v>
+      </c>
+      <c r="D59">
+        <v>0.52454527255029104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60">
+        <v>527765.86974000395</v>
+      </c>
+      <c r="C60" s="12">
+        <v>92685377289.217407</v>
+      </c>
+      <c r="D60">
+        <v>304442.732363933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>